<commit_message>
updated data and csv without BOM
</commit_message>
<xml_diff>
--- a/csp-guru/csp-guru.xlsx
+++ b/csp-guru/csp-guru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RTH\Documents\GitHub\csp-guru\csp-guru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A874F69D-7EF5-4D57-9CA5-EBD60AC25F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD50664F-75E1-4DBF-8440-F0283001899A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15330" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{CBAE575A-07C4-4BF8-8763-A77EB57639B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CBAE575A-07C4-4BF8-8763-A77EB57639B5}"/>
   </bookViews>
   <sheets>
     <sheet name="csp-guru" sheetId="2" r:id="rId1"/>
@@ -4391,8 +4391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932C9696-B96D-4ED0-ACF8-5A8E00AFA897}">
   <dimension ref="A1:DB148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G141" sqref="G141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33787,7 +33787,9 @@
       <c r="AY141" s="1"/>
       <c r="AZ141" s="1"/>
       <c r="BA141" s="1"/>
-      <c r="BB141" s="1"/>
+      <c r="BB141" s="1">
+        <v>12</v>
+      </c>
       <c r="BC141" s="1" t="s">
         <v>605</v>
       </c>

</xml_diff>

<commit_message>
deleted extra rows and colls
</commit_message>
<xml_diff>
--- a/csp-guru/csp-guru.xlsx
+++ b/csp-guru/csp-guru.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RTH\Documents\GitHub\csp-guru\csp-guru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD50664F-75E1-4DBF-8440-F0283001899A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E26CEBB-1DAC-4D4A-A62B-3B3D9278067D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CBAE575A-07C4-4BF8-8763-A77EB57639B5}"/>
   </bookViews>
@@ -3691,25 +3691,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -3727,14 +3714,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4389,10 +4375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932C9696-B96D-4ED0-ACF8-5A8E00AFA897}">
-  <dimension ref="A1:DB148"/>
+  <dimension ref="A1:CI145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G141" sqref="G141"/>
+    <sheetView tabSelected="1" topLeftCell="CF1" workbookViewId="0">
+      <selection activeCell="CJ1" sqref="CJ1:CS1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31555,7 +31541,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="129" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>1101</v>
       </c>
@@ -31737,7 +31723,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>1106</v>
       </c>
@@ -31916,7 +31902,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="131" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>1116</v>
       </c>
@@ -32089,7 +32075,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="132" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>1123</v>
       </c>
@@ -32253,7 +32239,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="133" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>1132</v>
       </c>
@@ -32429,7 +32415,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="134" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>1137</v>
       </c>
@@ -32593,7 +32579,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="135" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>1138</v>
       </c>
@@ -32757,7 +32743,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="136" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>1142</v>
       </c>
@@ -32930,7 +32916,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="137" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>1144</v>
       </c>
@@ -33097,7 +33083,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="138" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>1146</v>
       </c>
@@ -33291,27 +33277,8 @@
       <c r="CI138" s="1" t="s">
         <v>1149</v>
       </c>
-      <c r="CJ138" s="1"/>
-      <c r="CK138" s="1"/>
-      <c r="CL138" s="1"/>
-      <c r="CM138" s="1"/>
-      <c r="CN138" s="1"/>
-      <c r="CO138" s="1"/>
-      <c r="CP138" s="1"/>
-      <c r="CQ138" s="1"/>
-      <c r="CR138" s="1"/>
-      <c r="CS138" s="1"/>
-      <c r="CT138" s="1"/>
-      <c r="CU138" s="1"/>
-      <c r="CV138" s="1"/>
-      <c r="CW138" s="1"/>
-      <c r="CX138" s="1"/>
-      <c r="CY138" s="1"/>
-      <c r="CZ138" s="1"/>
-      <c r="DA138" s="1"/>
-      <c r="DB138" s="1"/>
     </row>
-    <row r="139" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>1150</v>
       </c>
@@ -33517,27 +33484,8 @@
       <c r="CI139" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CJ139" s="1"/>
-      <c r="CK139" s="1"/>
-      <c r="CL139" s="1"/>
-      <c r="CM139" s="1"/>
-      <c r="CN139" s="1"/>
-      <c r="CO139" s="1"/>
-      <c r="CP139" s="1"/>
-      <c r="CQ139" s="1"/>
-      <c r="CR139" s="1"/>
-      <c r="CS139" s="1"/>
-      <c r="CT139" s="1"/>
-      <c r="CU139" s="1"/>
-      <c r="CV139" s="1"/>
-      <c r="CW139" s="1"/>
-      <c r="CX139" s="1"/>
-      <c r="CY139" s="1"/>
-      <c r="CZ139" s="1"/>
-      <c r="DA139" s="1"/>
-      <c r="DB139" s="1"/>
     </row>
-    <row r="140" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>1180</v>
       </c>
@@ -33677,27 +33625,8 @@
       <c r="CI140" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="CJ140" s="1"/>
-      <c r="CK140" s="1"/>
-      <c r="CL140" s="1"/>
-      <c r="CM140" s="1"/>
-      <c r="CN140" s="1"/>
-      <c r="CO140" s="1"/>
-      <c r="CP140" s="1"/>
-      <c r="CQ140" s="1"/>
-      <c r="CR140" s="1"/>
-      <c r="CS140" s="1"/>
-      <c r="CT140" s="1"/>
-      <c r="CU140" s="1"/>
-      <c r="CV140" s="1"/>
-      <c r="CW140" s="1"/>
-      <c r="CX140" s="1"/>
-      <c r="CY140" s="1"/>
-      <c r="CZ140" s="1"/>
-      <c r="DA140" s="1"/>
-      <c r="DB140" s="1"/>
     </row>
-    <row r="141" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>1158</v>
       </c>
@@ -33831,27 +33760,8 @@
       <c r="CI141" s="1" t="s">
         <v>1171</v>
       </c>
-      <c r="CJ141" s="1"/>
-      <c r="CK141" s="1"/>
-      <c r="CL141" s="1"/>
-      <c r="CM141" s="1"/>
-      <c r="CN141" s="1"/>
-      <c r="CO141" s="1"/>
-      <c r="CP141" s="1"/>
-      <c r="CQ141" s="1"/>
-      <c r="CR141" s="1"/>
-      <c r="CS141" s="1"/>
-      <c r="CT141" s="1"/>
-      <c r="CU141" s="1"/>
-      <c r="CV141" s="1"/>
-      <c r="CW141" s="1"/>
-      <c r="CX141" s="1"/>
-      <c r="CY141" s="1"/>
-      <c r="CZ141" s="1"/>
-      <c r="DA141" s="1"/>
-      <c r="DB141" s="1"/>
     </row>
-    <row r="142" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>1200</v>
       </c>
@@ -33985,27 +33895,8 @@
       <c r="CI142" s="1" t="s">
         <v>1168</v>
       </c>
-      <c r="CJ142" s="1"/>
-      <c r="CK142" s="1"/>
-      <c r="CL142" s="1"/>
-      <c r="CM142" s="1"/>
-      <c r="CN142" s="1"/>
-      <c r="CO142" s="1"/>
-      <c r="CP142" s="1"/>
-      <c r="CQ142" s="1"/>
-      <c r="CR142" s="1"/>
-      <c r="CS142" s="1"/>
-      <c r="CT142" s="1"/>
-      <c r="CU142" s="1"/>
-      <c r="CV142" s="1"/>
-      <c r="CW142" s="1"/>
-      <c r="CX142" s="1"/>
-      <c r="CY142" s="1"/>
-      <c r="CZ142" s="1"/>
-      <c r="DA142" s="1"/>
-      <c r="DB142" s="1"/>
     </row>
-    <row r="143" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>1201</v>
       </c>
@@ -34165,27 +34056,8 @@
       <c r="CI143" s="1" t="s">
         <v>1185</v>
       </c>
-      <c r="CJ143" s="1"/>
-      <c r="CK143" s="1"/>
-      <c r="CL143" s="1"/>
-      <c r="CM143" s="1"/>
-      <c r="CN143" s="1"/>
-      <c r="CO143" s="1"/>
-      <c r="CP143" s="1"/>
-      <c r="CQ143" s="1"/>
-      <c r="CR143" s="1"/>
-      <c r="CS143" s="1"/>
-      <c r="CT143" s="1"/>
-      <c r="CU143" s="1"/>
-      <c r="CV143" s="1"/>
-      <c r="CW143" s="1"/>
-      <c r="CX143" s="1"/>
-      <c r="CY143" s="1"/>
-      <c r="CZ143" s="1"/>
-      <c r="DA143" s="1"/>
-      <c r="DB143" s="1"/>
     </row>
-    <row r="144" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>1186</v>
       </c>
@@ -34298,7 +34170,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="145" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>1198</v>
       </c>
@@ -34323,7 +34195,7 @@
       <c r="N145" t="s">
         <v>1189</v>
       </c>
-      <c r="Q145" s="4">
+      <c r="Q145" s="3">
         <v>1800</v>
       </c>
       <c r="AL145" t="s">
@@ -34347,222 +34219,6 @@
       <c r="BP145" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="147" spans="1:106" x14ac:dyDescent="0.25">
-      <c r="A147" s="3"/>
-      <c r="B147" s="1"/>
-      <c r="C147" s="1"/>
-      <c r="D147" s="1"/>
-      <c r="E147" s="1"/>
-      <c r="F147" s="1"/>
-      <c r="G147" s="1"/>
-      <c r="H147" s="1"/>
-      <c r="I147" s="1"/>
-      <c r="J147" s="1"/>
-      <c r="K147" s="1"/>
-      <c r="L147" s="1"/>
-      <c r="M147" s="1"/>
-      <c r="N147" s="1"/>
-      <c r="O147" s="1"/>
-      <c r="P147" s="1"/>
-      <c r="Q147" s="1"/>
-      <c r="R147" s="1"/>
-      <c r="S147" s="1"/>
-      <c r="T147" s="1"/>
-      <c r="U147" s="1"/>
-      <c r="V147" s="1"/>
-      <c r="W147" s="1"/>
-      <c r="X147" s="1"/>
-      <c r="Y147" s="1"/>
-      <c r="Z147" s="1"/>
-      <c r="AA147" s="1"/>
-      <c r="AB147" s="1"/>
-      <c r="AC147" s="1"/>
-      <c r="AD147" s="1"/>
-      <c r="AE147" s="1"/>
-      <c r="AF147" s="1"/>
-      <c r="AG147" s="1"/>
-      <c r="AH147" s="1"/>
-      <c r="AI147" s="1"/>
-      <c r="AJ147" s="1"/>
-      <c r="AK147" s="1"/>
-      <c r="AL147" s="1"/>
-      <c r="AM147" s="1"/>
-      <c r="AN147" s="1"/>
-      <c r="AO147" s="1"/>
-      <c r="AP147" s="1"/>
-      <c r="AQ147" s="1"/>
-      <c r="AR147" s="1"/>
-      <c r="AS147" s="1"/>
-      <c r="AT147" s="1"/>
-      <c r="AU147" s="1"/>
-      <c r="AV147" s="1"/>
-      <c r="AW147" s="1"/>
-      <c r="AX147" s="1"/>
-      <c r="AY147" s="1"/>
-      <c r="AZ147" s="1"/>
-      <c r="BA147" s="1"/>
-      <c r="BB147" s="1"/>
-      <c r="BC147" s="1"/>
-      <c r="BD147" s="1"/>
-      <c r="BE147" s="1"/>
-      <c r="BF147" s="1"/>
-      <c r="BG147" s="1"/>
-      <c r="BH147" s="1"/>
-      <c r="BI147" s="1"/>
-      <c r="BJ147" s="1"/>
-      <c r="BK147" s="1"/>
-      <c r="BL147" s="1"/>
-      <c r="BM147" s="1"/>
-      <c r="BN147" s="1"/>
-      <c r="BO147" s="1"/>
-      <c r="BP147" s="1"/>
-      <c r="BQ147" s="1"/>
-      <c r="BR147" s="1"/>
-      <c r="BS147" s="1"/>
-      <c r="BT147" s="1"/>
-      <c r="BU147" s="1"/>
-      <c r="BV147" s="1"/>
-      <c r="BW147" s="1"/>
-      <c r="BX147" s="1"/>
-      <c r="BY147" s="1"/>
-      <c r="BZ147" s="1"/>
-      <c r="CA147" s="1"/>
-      <c r="CB147" s="1"/>
-      <c r="CC147" s="1"/>
-      <c r="CD147" s="1"/>
-      <c r="CE147" s="1"/>
-      <c r="CF147" s="1"/>
-      <c r="CG147" s="1"/>
-      <c r="CH147" s="1"/>
-      <c r="CI147" s="1"/>
-      <c r="CJ147" s="1"/>
-      <c r="CK147" s="1"/>
-      <c r="CL147" s="1"/>
-      <c r="CM147" s="1"/>
-      <c r="CN147" s="1"/>
-      <c r="CO147" s="1"/>
-      <c r="CP147" s="1"/>
-      <c r="CQ147" s="1"/>
-      <c r="CR147" s="1"/>
-      <c r="CS147" s="1"/>
-      <c r="CT147" s="1"/>
-      <c r="CU147" s="1"/>
-      <c r="CV147" s="1"/>
-      <c r="CW147" s="1"/>
-      <c r="CX147" s="1"/>
-      <c r="CY147" s="1"/>
-      <c r="CZ147" s="1"/>
-      <c r="DA147" s="1"/>
-      <c r="DB147" s="1"/>
-    </row>
-    <row r="148" spans="1:106" x14ac:dyDescent="0.25">
-      <c r="A148" s="1"/>
-      <c r="B148" s="1"/>
-      <c r="C148" s="1"/>
-      <c r="D148" s="1"/>
-      <c r="E148" s="1"/>
-      <c r="F148" s="1"/>
-      <c r="G148" s="1"/>
-      <c r="H148" s="1"/>
-      <c r="I148" s="1"/>
-      <c r="J148" s="1"/>
-      <c r="K148" s="1"/>
-      <c r="L148" s="1"/>
-      <c r="M148" s="1"/>
-      <c r="N148" s="1"/>
-      <c r="O148" s="1"/>
-      <c r="P148" s="1"/>
-      <c r="Q148" s="1"/>
-      <c r="R148" s="1"/>
-      <c r="S148" s="1"/>
-      <c r="T148" s="1"/>
-      <c r="U148" s="1"/>
-      <c r="V148" s="1"/>
-      <c r="W148" s="1"/>
-      <c r="X148" s="1"/>
-      <c r="Y148" s="1"/>
-      <c r="Z148" s="1"/>
-      <c r="AA148" s="1"/>
-      <c r="AB148" s="1"/>
-      <c r="AC148" s="1"/>
-      <c r="AD148" s="1"/>
-      <c r="AE148" s="1"/>
-      <c r="AF148" s="1"/>
-      <c r="AG148" s="1"/>
-      <c r="AH148" s="1"/>
-      <c r="AI148" s="1"/>
-      <c r="AJ148" s="1"/>
-      <c r="AK148" s="1"/>
-      <c r="AL148" s="1"/>
-      <c r="AM148" s="1"/>
-      <c r="AN148" s="1"/>
-      <c r="AO148" s="1"/>
-      <c r="AP148" s="1"/>
-      <c r="AQ148" s="1"/>
-      <c r="AR148" s="1"/>
-      <c r="AS148" s="1"/>
-      <c r="AT148" s="1"/>
-      <c r="AU148" s="1"/>
-      <c r="AV148" s="1"/>
-      <c r="AW148" s="1"/>
-      <c r="AX148" s="1"/>
-      <c r="AY148" s="1"/>
-      <c r="AZ148" s="1"/>
-      <c r="BA148" s="1"/>
-      <c r="BB148" s="1"/>
-      <c r="BC148" s="1"/>
-      <c r="BD148" s="1"/>
-      <c r="BE148" s="1"/>
-      <c r="BF148" s="1"/>
-      <c r="BG148" s="1"/>
-      <c r="BH148" s="1"/>
-      <c r="BI148" s="1"/>
-      <c r="BJ148" s="1"/>
-      <c r="BK148" s="1"/>
-      <c r="BL148" s="1"/>
-      <c r="BM148" s="1"/>
-      <c r="BN148" s="1"/>
-      <c r="BO148" s="1"/>
-      <c r="BP148" s="1"/>
-      <c r="BQ148" s="1"/>
-      <c r="BR148" s="1"/>
-      <c r="BS148" s="1"/>
-      <c r="BT148" s="1"/>
-      <c r="BU148" s="1"/>
-      <c r="BV148" s="1"/>
-      <c r="BW148" s="1"/>
-      <c r="BX148" s="1"/>
-      <c r="BY148" s="1"/>
-      <c r="BZ148" s="1"/>
-      <c r="CA148" s="1"/>
-      <c r="CB148" s="1"/>
-      <c r="CC148" s="1"/>
-      <c r="CD148" s="1"/>
-      <c r="CE148" s="1"/>
-      <c r="CF148" s="1"/>
-      <c r="CG148" s="1"/>
-      <c r="CH148" s="1"/>
-      <c r="CI148" s="1"/>
-      <c r="CJ148" s="1"/>
-      <c r="CK148" s="1"/>
-      <c r="CL148" s="1"/>
-      <c r="CM148" s="1"/>
-      <c r="CN148" s="1"/>
-      <c r="CO148" s="1"/>
-      <c r="CP148" s="1"/>
-      <c r="CQ148" s="1"/>
-      <c r="CR148" s="1"/>
-      <c r="CS148" s="1"/>
-      <c r="CT148" s="1"/>
-      <c r="CU148" s="1"/>
-      <c r="CV148" s="1"/>
-      <c r="CW148" s="1"/>
-      <c r="CX148" s="1"/>
-      <c r="CY148" s="1"/>
-      <c r="CZ148" s="1"/>
-      <c r="DA148" s="1"/>
-      <c r="DB148" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>